<commit_message>
data update - 22 aug
</commit_message>
<xml_diff>
--- a/data/ptypes_dump.xlsx
+++ b/data/ptypes_dump.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amida\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7A99E36-691C-4FB1-BCC5-E954C6017956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF7A8B85-B8F3-410A-9D6B-2EAF18D090E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18150,9 +18150,7 @@
   </sheetPr>
   <dimension ref="A1:B5954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2818" workbookViewId="0">
-      <selection activeCell="B2831" sqref="B2831"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
data update - sept 1
</commit_message>
<xml_diff>
--- a/data/ptypes_dump.xlsx
+++ b/data/ptypes_dump.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amida\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adarsh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF7A8B85-B8F3-410A-9D6B-2EAF18D090E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{718F42B3-7047-4AB4-AAD9-F5A872761904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
data update - sept 6
</commit_message>
<xml_diff>
--- a/data/ptypes_dump.xlsx
+++ b/data/ptypes_dump.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adarsh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{718F42B3-7047-4AB4-AAD9-F5A872761904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{685074A9-4518-44FE-9BC9-B49159A84324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
10 sept data update
</commit_message>
<xml_diff>
--- a/data/ptypes_dump.xlsx
+++ b/data/ptypes_dump.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29301"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adarsh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{685074A9-4518-44FE-9BC9-B49159A84324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C0CD525-984B-49F1-ABAF-3FBCA5B21542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PTypes Dump" sheetId="6" r:id="rId1"/>
+    <sheet name="PTypes Dump" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -18144,7 +18144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>